<commit_message>
Done create new offer
</commit_message>
<xml_diff>
--- a/data/mock-data.xlsx
+++ b/data/mock-data.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bes/cc18/Project/Swapy02/server/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{608DD266-A6B2-594C-8BD6-E696EF071255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA86449F-C9C7-D945-B3D6-4453BDFA4E3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5720" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{EBC99A39-14E9-FD43-AB84-C80166CFC4A2}"/>
+    <workbookView xWindow="-5720" yWindow="-21100" windowWidth="38400" windowHeight="21100" activeTab="4" xr2:uid="{EBC99A39-14E9-FD43-AB84-C80166CFC4A2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Offer" sheetId="10" r:id="rId1"/>
-    <sheet name="User" sheetId="21" r:id="rId2"/>
-    <sheet name="Asset" sheetId="22" r:id="rId3"/>
-    <sheet name="Asset_Pic" sheetId="8" r:id="rId4"/>
+    <sheet name="User" sheetId="21" r:id="rId1"/>
+    <sheet name="Asset" sheetId="22" r:id="rId2"/>
+    <sheet name="Asset_Pic" sheetId="8" r:id="rId3"/>
+    <sheet name="Offer" sheetId="10" r:id="rId4"/>
     <sheet name="Offer_Asset" sheetId="11" r:id="rId5"/>
     <sheet name="Message" sheetId="12" r:id="rId6"/>
     <sheet name="ENUM" sheetId="9" r:id="rId7"/>
@@ -25,7 +25,8 @@
     <sheet name="Issue" sheetId="26" r:id="rId10"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Asset!$A$1:$N$195</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Asset!$A$1:$N$195</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Offer_Asset!$A$1:$K$16</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -4212,218 +4213,6 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97A7A880-88D7-644F-A393-17F364CA67FC}">
-  <sheetPr>
-    <tabColor rgb="FFFFC000"/>
-  </sheetPr>
-  <dimension ref="A1:I5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="109" workbookViewId="0">
-      <selection activeCell="N26" sqref="N26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="10.83203125" style="4"/>
-    <col min="2" max="3" width="10.83203125" style="7"/>
-    <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="10.83203125" style="4"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
-        <v>545</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>624</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>625</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>546</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>547</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>548</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>1243</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>1244</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="10">
-        <v>1</v>
-      </c>
-      <c r="B2" s="7">
-        <v>45555.268175578705</v>
-      </c>
-      <c r="C2" s="7">
-        <v>45555.268175578705</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>553</v>
-      </c>
-      <c r="E2" s="10">
-        <v>2</v>
-      </c>
-      <c r="F2" s="10">
-        <v>3</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>1226</v>
-      </c>
-      <c r="H2" s="3">
-        <v>0</v>
-      </c>
-      <c r="I2" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="10">
-        <v>2</v>
-      </c>
-      <c r="B3" s="7">
-        <v>45555.268175578705</v>
-      </c>
-      <c r="C3" s="7">
-        <v>45555.268175578705</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>1223</v>
-      </c>
-      <c r="E3" s="10">
-        <v>2</v>
-      </c>
-      <c r="F3" s="10">
-        <v>4</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>1227</v>
-      </c>
-      <c r="H3" s="3">
-        <v>1</v>
-      </c>
-      <c r="I3" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="10">
-        <v>3</v>
-      </c>
-      <c r="B4" s="7">
-        <v>45555.268175578705</v>
-      </c>
-      <c r="C4" s="7">
-        <v>45555.268175578705</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>1224</v>
-      </c>
-      <c r="E4" s="10">
-        <v>2</v>
-      </c>
-      <c r="F4" s="10">
-        <v>5</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>1228</v>
-      </c>
-      <c r="H4" s="3">
-        <v>1</v>
-      </c>
-      <c r="I4" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="10">
-        <v>4</v>
-      </c>
-      <c r="B5" s="7">
-        <v>45555.268175578705</v>
-      </c>
-      <c r="C5" s="7">
-        <v>45555.268175578705</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>1225</v>
-      </c>
-      <c r="E5" s="10">
-        <v>5</v>
-      </c>
-      <c r="F5" s="10">
-        <v>2</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>1226</v>
-      </c>
-      <c r="H5" s="3">
-        <v>0</v>
-      </c>
-      <c r="I5" s="3">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48BCAA29-5AE5-7B49-B807-BAA244DF2D78}">
-  <sheetPr>
-    <tabColor rgb="FFFFC000"/>
-  </sheetPr>
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="3" max="3" width="23.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>681</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1241</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1229</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1233</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1242</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B15C52B3-B937-EF4D-B5E6-C10059C00188}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -5446,15 +5235,58 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48BCAA29-5AE5-7B49-B807-BAA244DF2D78}">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="23.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>681</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1241</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1229</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1233</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60A717BA-F36B-C649-B9AA-87E2D76B1937}">
-  <sheetPr>
+  <sheetPr filterMode="1">
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
   <dimension ref="A1:P195"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="D132" sqref="D132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5462,6 +5294,7 @@
     <col min="1" max="1" width="10.83203125" style="6"/>
     <col min="2" max="3" width="10.83203125" style="7"/>
     <col min="4" max="4" width="10.83203125" style="6"/>
+    <col min="5" max="5" width="37.83203125" customWidth="1"/>
     <col min="9" max="9" width="83.83203125" customWidth="1"/>
     <col min="10" max="10" width="50.5" customWidth="1"/>
     <col min="12" max="15" width="10.83203125" style="4"/>
@@ -5517,7 +5350,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -5564,7 +5397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -5611,7 +5444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -5658,7 +5491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -5705,7 +5538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -5752,7 +5585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -5799,7 +5632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -5846,7 +5679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -5893,7 +5726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -5940,7 +5773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
         <v>10</v>
       </c>
@@ -5987,7 +5820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
         <v>11</v>
       </c>
@@ -6034,7 +5867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6">
         <v>12</v>
       </c>
@@ -6131,7 +5964,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
         <v>14</v>
       </c>
@@ -6178,7 +6011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
         <v>15</v>
       </c>
@@ -6225,7 +6058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="6">
         <v>16</v>
       </c>
@@ -6269,7 +6102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="6">
         <v>17</v>
       </c>
@@ -6313,7 +6146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="6">
         <v>18</v>
       </c>
@@ -6357,7 +6190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
         <v>19</v>
       </c>
@@ -6401,7 +6234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="6">
         <v>20</v>
       </c>
@@ -6445,7 +6278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
         <v>21</v>
       </c>
@@ -6489,7 +6322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="6">
         <v>22</v>
       </c>
@@ -6533,7 +6366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
         <v>23</v>
       </c>
@@ -6577,7 +6410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="6">
         <v>24</v>
       </c>
@@ -6621,7 +6454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="6">
         <v>25</v>
       </c>
@@ -6665,7 +6498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="6">
         <v>26</v>
       </c>
@@ -6709,7 +6542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="6">
         <v>27</v>
       </c>
@@ -6753,7 +6586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="6">
         <v>28</v>
       </c>
@@ -6797,7 +6630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="6">
         <v>29</v>
       </c>
@@ -6841,7 +6674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="6">
         <v>30</v>
       </c>
@@ -6885,7 +6718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="6">
         <v>31</v>
       </c>
@@ -6929,7 +6762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="6">
         <v>32</v>
       </c>
@@ -6973,7 +6806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="6">
         <v>33</v>
       </c>
@@ -7017,7 +6850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="6">
         <v>34</v>
       </c>
@@ -7061,7 +6894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="6">
         <v>35</v>
       </c>
@@ -7105,7 +6938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="6">
         <v>36</v>
       </c>
@@ -7149,7 +6982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="6">
         <v>37</v>
       </c>
@@ -7193,7 +7026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="6">
         <v>38</v>
       </c>
@@ -7237,7 +7070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="6">
         <v>39</v>
       </c>
@@ -7281,7 +7114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="6">
         <v>40</v>
       </c>
@@ -7325,7 +7158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="6">
         <v>41</v>
       </c>
@@ -7369,7 +7202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="6">
         <v>42</v>
       </c>
@@ -7413,7 +7246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="6">
         <v>43</v>
       </c>
@@ -7457,7 +7290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="6">
         <v>44</v>
       </c>
@@ -7501,7 +7334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="6">
         <v>45</v>
       </c>
@@ -7545,7 +7378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="6">
         <v>46</v>
       </c>
@@ -7589,7 +7422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="6">
         <v>47</v>
       </c>
@@ -7633,7 +7466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="6">
         <v>48</v>
       </c>
@@ -7677,7 +7510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="6">
         <v>49</v>
       </c>
@@ -7721,7 +7554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="6">
         <v>50</v>
       </c>
@@ -7765,7 +7598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="6">
         <v>51</v>
       </c>
@@ -7809,7 +7642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="6">
         <v>52</v>
       </c>
@@ -7853,7 +7686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="6">
         <v>53</v>
       </c>
@@ -7897,7 +7730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="6">
         <v>54</v>
       </c>
@@ -7941,7 +7774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="6">
         <v>55</v>
       </c>
@@ -7985,7 +7818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="6">
         <v>56</v>
       </c>
@@ -8029,7 +7862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="6">
         <v>57</v>
       </c>
@@ -8073,7 +7906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="6">
         <v>58</v>
       </c>
@@ -8117,7 +7950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="6">
         <v>59</v>
       </c>
@@ -8161,7 +7994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="6">
         <v>60</v>
       </c>
@@ -8205,7 +8038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="6">
         <v>61</v>
       </c>
@@ -8249,7 +8082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="6">
         <v>62</v>
       </c>
@@ -8293,7 +8126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="6">
         <v>63</v>
       </c>
@@ -8337,7 +8170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="6">
         <v>64</v>
       </c>
@@ -8381,7 +8214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="6">
         <v>65</v>
       </c>
@@ -8425,7 +8258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="6">
         <v>66</v>
       </c>
@@ -8469,7 +8302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="6">
         <v>67</v>
       </c>
@@ -8513,7 +8346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="6">
         <v>68</v>
       </c>
@@ -8557,7 +8390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="6">
         <v>69</v>
       </c>
@@ -8601,7 +8434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="6">
         <v>70</v>
       </c>
@@ -8645,7 +8478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" s="6">
         <v>71</v>
       </c>
@@ -8689,7 +8522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" s="6">
         <v>72</v>
       </c>
@@ -8733,7 +8566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="6">
         <v>73</v>
       </c>
@@ -8777,7 +8610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="6">
         <v>74</v>
       </c>
@@ -8821,7 +8654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="6">
         <v>75</v>
       </c>
@@ -8865,7 +8698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="6">
         <v>76</v>
       </c>
@@ -8909,7 +8742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="6">
         <v>77</v>
       </c>
@@ -8953,7 +8786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="6">
         <v>78</v>
       </c>
@@ -9000,7 +8833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="6">
         <v>79</v>
       </c>
@@ -9047,7 +8880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="6">
         <v>80</v>
       </c>
@@ -9094,7 +8927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="6">
         <v>81</v>
       </c>
@@ -9141,7 +8974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" s="6">
         <v>82</v>
       </c>
@@ -9188,7 +9021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" s="6">
         <v>83</v>
       </c>
@@ -9235,7 +9068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" s="6">
         <v>84</v>
       </c>
@@ -9282,7 +9115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" s="6">
         <v>85</v>
       </c>
@@ -9329,7 +9162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" s="6">
         <v>86</v>
       </c>
@@ -9376,7 +9209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" s="6">
         <v>87</v>
       </c>
@@ -9423,7 +9256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" s="6">
         <v>88</v>
       </c>
@@ -9470,7 +9303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" s="6">
         <v>89</v>
       </c>
@@ -9517,7 +9350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" s="6">
         <v>90</v>
       </c>
@@ -9564,7 +9397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" s="6">
         <v>91</v>
       </c>
@@ -9611,7 +9444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" s="6">
         <v>92</v>
       </c>
@@ -9658,7 +9491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" s="6">
         <v>93</v>
       </c>
@@ -9705,7 +9538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" s="6">
         <v>94</v>
       </c>
@@ -9752,7 +9585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" s="6">
         <v>95</v>
       </c>
@@ -9799,7 +9632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" s="6">
         <v>96</v>
       </c>
@@ -9846,7 +9679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" s="6">
         <v>97</v>
       </c>
@@ -9893,7 +9726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" s="6">
         <v>98</v>
       </c>
@@ -9940,7 +9773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" s="6">
         <v>99</v>
       </c>
@@ -9987,7 +9820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" s="6">
         <v>100</v>
       </c>
@@ -10034,7 +9867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" s="6">
         <v>101</v>
       </c>
@@ -10081,7 +9914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" s="6">
         <v>102</v>
       </c>
@@ -10128,7 +9961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" s="6">
         <v>103</v>
       </c>
@@ -10175,7 +10008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" s="6">
         <v>104</v>
       </c>
@@ -10222,7 +10055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" s="6">
         <v>105</v>
       </c>
@@ -10269,7 +10102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" s="6">
         <v>106</v>
       </c>
@@ -10316,7 +10149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" s="6">
         <v>107</v>
       </c>
@@ -10363,7 +10196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" s="6">
         <v>108</v>
       </c>
@@ -10410,7 +10243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" s="6">
         <v>109</v>
       </c>
@@ -10457,7 +10290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" s="6">
         <v>110</v>
       </c>
@@ -10504,7 +10337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" s="6">
         <v>111</v>
       </c>
@@ -10551,7 +10384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" s="6">
         <v>112</v>
       </c>
@@ -10598,7 +10431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" s="6">
         <v>113</v>
       </c>
@@ -10645,7 +10478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" s="6">
         <v>114</v>
       </c>
@@ -10692,7 +10525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" s="6">
         <v>115</v>
       </c>
@@ -10739,7 +10572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" s="6">
         <v>116</v>
       </c>
@@ -10786,7 +10619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" s="6">
         <v>117</v>
       </c>
@@ -10833,7 +10666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" s="6">
         <v>118</v>
       </c>
@@ -10880,7 +10713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" s="6">
         <v>119</v>
       </c>
@@ -10927,7 +10760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" s="6">
         <v>120</v>
       </c>
@@ -10974,7 +10807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" s="6">
         <v>121</v>
       </c>
@@ -11021,7 +10854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" s="6">
         <v>122</v>
       </c>
@@ -11068,7 +10901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" s="6">
         <v>123</v>
       </c>
@@ -11115,7 +10948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" s="6">
         <v>124</v>
       </c>
@@ -11162,7 +10995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" s="6">
         <v>125</v>
       </c>
@@ -11209,7 +11042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" s="6">
         <v>126</v>
       </c>
@@ -11256,7 +11089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" s="6">
         <v>127</v>
       </c>
@@ -11303,7 +11136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" s="6">
         <v>128</v>
       </c>
@@ -11350,7 +11183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" s="6">
         <v>129</v>
       </c>
@@ -11397,7 +11230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" s="6">
         <v>130</v>
       </c>
@@ -11494,7 +11327,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="133" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" s="6">
         <v>132</v>
       </c>
@@ -11541,7 +11374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" s="6">
         <v>133</v>
       </c>
@@ -11588,7 +11421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" s="6">
         <v>134</v>
       </c>
@@ -11635,7 +11468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" s="6">
         <v>135</v>
       </c>
@@ -11682,7 +11515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" s="6">
         <v>136</v>
       </c>
@@ -11776,7 +11609,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="139" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" s="6">
         <v>138</v>
       </c>
@@ -11820,7 +11653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" s="6">
         <v>139</v>
       </c>
@@ -11911,7 +11744,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="142" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142" s="6">
         <v>141</v>
       </c>
@@ -11955,7 +11788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" s="6">
         <v>142</v>
       </c>
@@ -11999,7 +11832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144" s="6">
         <v>143</v>
       </c>
@@ -12043,7 +11876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145" s="6">
         <v>144</v>
       </c>
@@ -12087,7 +11920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146" s="6">
         <v>145</v>
       </c>
@@ -12131,7 +11964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147" s="6">
         <v>146</v>
       </c>
@@ -12175,7 +12008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148" s="6">
         <v>147</v>
       </c>
@@ -12219,7 +12052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149" s="6">
         <v>148</v>
       </c>
@@ -12263,7 +12096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A150" s="6">
         <v>149</v>
       </c>
@@ -12307,7 +12140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A151" s="6">
         <v>150</v>
       </c>
@@ -12351,7 +12184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A152" s="6">
         <v>151</v>
       </c>
@@ -12395,7 +12228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A153" s="6">
         <v>152</v>
       </c>
@@ -12439,7 +12272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A154" s="6">
         <v>153</v>
       </c>
@@ -12483,7 +12316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A155" s="6">
         <v>154</v>
       </c>
@@ -12530,7 +12363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A156" s="6">
         <v>155</v>
       </c>
@@ -12577,7 +12410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A157" s="6">
         <v>156</v>
       </c>
@@ -12624,7 +12457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A158" s="6">
         <v>157</v>
       </c>
@@ -12671,7 +12504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A159" s="6">
         <v>158</v>
       </c>
@@ -12718,7 +12551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A160" s="6">
         <v>159</v>
       </c>
@@ -12765,7 +12598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A161" s="6">
         <v>160</v>
       </c>
@@ -12812,7 +12645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A162" s="6">
         <v>161</v>
       </c>
@@ -12859,7 +12692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A163" s="6">
         <v>162</v>
       </c>
@@ -12903,7 +12736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A164" s="6">
         <v>163</v>
       </c>
@@ -12947,7 +12780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A165" s="6">
         <v>164</v>
       </c>
@@ -12991,7 +12824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A166" s="6">
         <v>165</v>
       </c>
@@ -13035,7 +12868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A167" s="6">
         <v>166</v>
       </c>
@@ -13079,7 +12912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A168" s="6">
         <v>167</v>
       </c>
@@ -13126,7 +12959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A169" s="6">
         <v>168</v>
       </c>
@@ -13173,7 +13006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A170" s="6">
         <v>169</v>
       </c>
@@ -13220,7 +13053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A171" s="6">
         <v>170</v>
       </c>
@@ -13267,7 +13100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A172" s="6">
         <v>171</v>
       </c>
@@ -13314,7 +13147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A173" s="6">
         <v>172</v>
       </c>
@@ -13361,7 +13194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A174" s="6">
         <v>173</v>
       </c>
@@ -13408,7 +13241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A175" s="6">
         <v>174</v>
       </c>
@@ -13455,7 +13288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A176" s="6">
         <v>175</v>
       </c>
@@ -13502,7 +13335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A177" s="6">
         <v>176</v>
       </c>
@@ -13549,7 +13382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A178" s="6">
         <v>177</v>
       </c>
@@ -13593,7 +13426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A179" s="6">
         <v>178</v>
       </c>
@@ -13637,7 +13470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A180" s="6">
         <v>179</v>
       </c>
@@ -13681,7 +13514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A181" s="6">
         <v>180</v>
       </c>
@@ -13725,7 +13558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A182" s="6">
         <v>181</v>
       </c>
@@ -13769,7 +13602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A183" s="6">
         <v>182</v>
       </c>
@@ -13813,7 +13646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A184" s="6">
         <v>183</v>
       </c>
@@ -13857,7 +13690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A185" s="6">
         <v>184</v>
       </c>
@@ -13901,7 +13734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A186" s="6">
         <v>185</v>
       </c>
@@ -13948,7 +13781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A187" s="6">
         <v>186</v>
       </c>
@@ -13995,7 +13828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A188" s="6">
         <v>187</v>
       </c>
@@ -14042,7 +13875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A189" s="6">
         <v>188</v>
       </c>
@@ -14089,7 +13922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A190" s="6">
         <v>189</v>
       </c>
@@ -14136,7 +13969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A191" s="6">
         <v>190</v>
       </c>
@@ -14183,7 +14016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A192" s="6">
         <v>191</v>
       </c>
@@ -14230,7 +14063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A193" s="6">
         <v>192</v>
       </c>
@@ -14277,7 +14110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A194" s="6">
         <v>193</v>
       </c>
@@ -14324,7 +14157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A195" s="6">
         <v>194</v>
       </c>
@@ -14372,7 +14205,15 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N195" xr:uid="{60A717BA-F36B-C649-B9AA-87E2D76B1937}"/>
+  <autoFilter ref="A1:N195" xr:uid="{60A717BA-F36B-C649-B9AA-87E2D76B1937}">
+    <filterColumn colId="10">
+      <filters>
+        <filter val="MATCHED"/>
+        <filter val="RECEIVED"/>
+        <filter val="SHIPPED"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <hyperlinks>
     <hyperlink ref="J2" r:id="rId1" display="https://cdn.dummyjson.com/products/images/beauty/Essence%20Mascara%20Lash%20Princess/1.png" xr:uid="{0C52951E-CA4F-6C4B-98A7-082640BBB772}"/>
   </hyperlinks>
@@ -14380,7 +14221,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9791BC7D-8D17-FF4C-8AD6-DF0307A2C1F5}">
   <sheetPr codeName="Sheet8">
     <tabColor rgb="FFFFC000"/>
@@ -24381,15 +24222,184 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97A7A880-88D7-644F-A393-17F364CA67FC}">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="A1:I5"/>
+  <sheetViews>
+    <sheetView zoomScale="109" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="4"/>
+    <col min="2" max="3" width="10.83203125" style="7"/>
+    <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.83203125" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>545</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>624</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>625</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>546</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>547</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>548</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>1243</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>1244</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="10">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7">
+        <v>45555.268175578705</v>
+      </c>
+      <c r="C2" s="7">
+        <v>45555.268175578705</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>553</v>
+      </c>
+      <c r="E2" s="10">
+        <v>2</v>
+      </c>
+      <c r="F2" s="10">
+        <v>3</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>1226</v>
+      </c>
+      <c r="H2" s="3">
+        <v>0</v>
+      </c>
+      <c r="I2" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="10">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7">
+        <v>45555.268175578705</v>
+      </c>
+      <c r="C3" s="7">
+        <v>45555.268175578705</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>1223</v>
+      </c>
+      <c r="E3" s="10">
+        <v>2</v>
+      </c>
+      <c r="F3" s="10">
+        <v>4</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>1227</v>
+      </c>
+      <c r="H3" s="3">
+        <v>1</v>
+      </c>
+      <c r="I3" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="10">
+        <v>3</v>
+      </c>
+      <c r="B4" s="7">
+        <v>45555.268175578705</v>
+      </c>
+      <c r="C4" s="7">
+        <v>45555.268175578705</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>1224</v>
+      </c>
+      <c r="E4" s="10">
+        <v>2</v>
+      </c>
+      <c r="F4" s="10">
+        <v>5</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>1228</v>
+      </c>
+      <c r="H4" s="3">
+        <v>1</v>
+      </c>
+      <c r="I4" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="10">
+        <v>4</v>
+      </c>
+      <c r="B5" s="7">
+        <v>45555.268175578705</v>
+      </c>
+      <c r="C5" s="7">
+        <v>45555.268175578705</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>1225</v>
+      </c>
+      <c r="E5" s="10">
+        <v>5</v>
+      </c>
+      <c r="F5" s="10">
+        <v>2</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>1226</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0</v>
+      </c>
+      <c r="I5" s="3">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75DA7273-E739-C44B-8EA5-04AF4A472D36}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -24400,7 +24410,7 @@
     <col min="5" max="5" width="23.1640625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>554</v>
       </c>
@@ -24417,7 +24427,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -24433,12 +24443,8 @@
       <c r="E2" s="4">
         <v>19</v>
       </c>
-      <c r="F2">
-        <f>VLOOKUP(E2,Asset!A:D,4,FALSE)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -24454,12 +24460,8 @@
       <c r="E3" s="4">
         <v>73</v>
       </c>
-      <c r="F3">
-        <f>VLOOKUP(E3,Asset!A:D,4,FALSE)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -24475,12 +24477,8 @@
       <c r="E4" s="4">
         <v>11</v>
       </c>
-      <c r="F4">
-        <f>VLOOKUP(E4,Asset!A:D,4,FALSE)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -24496,12 +24494,8 @@
       <c r="E5" s="4">
         <v>24</v>
       </c>
-      <c r="F5">
-        <f>VLOOKUP(E5,Asset!A:D,4,FALSE)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -24517,12 +24511,8 @@
       <c r="E6" s="4">
         <v>34</v>
       </c>
-      <c r="F6">
-        <f>VLOOKUP(E6,Asset!A:D,4,FALSE)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -24538,12 +24528,8 @@
       <c r="E7" s="9">
         <v>131</v>
       </c>
-      <c r="F7">
-        <f>VLOOKUP(E7,Asset!A:D,4,FALSE)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -24559,12 +24545,8 @@
       <c r="E8" s="9">
         <v>137</v>
       </c>
-      <c r="F8">
-        <f>VLOOKUP(E8,Asset!A:D,4,FALSE)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -24580,12 +24562,8 @@
       <c r="E9" s="9">
         <v>140</v>
       </c>
-      <c r="F9">
-        <f>VLOOKUP(E9,Asset!A:D,4,FALSE)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -24601,12 +24579,8 @@
       <c r="E10" s="9">
         <v>13</v>
       </c>
-      <c r="F10">
-        <f>VLOOKUP(E10,Asset!A:D,4,FALSE)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -24622,12 +24596,8 @@
       <c r="E11" s="9">
         <v>131</v>
       </c>
-      <c r="F11">
-        <f>VLOOKUP(E11,Asset!A:D,4,FALSE)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -24643,12 +24613,8 @@
       <c r="E12" s="4">
         <v>45</v>
       </c>
-      <c r="F12">
-        <f>VLOOKUP(E12,Asset!A:D,4,FALSE)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -24664,12 +24630,8 @@
       <c r="E13" s="4">
         <v>47</v>
       </c>
-      <c r="F13">
-        <f>VLOOKUP(E13,Asset!A:D,4,FALSE)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -24685,12 +24647,8 @@
       <c r="E14" s="4">
         <v>144</v>
       </c>
-      <c r="F14">
-        <f>VLOOKUP(E14,Asset!A:D,4,FALSE)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -24706,12 +24664,8 @@
       <c r="E15" s="4">
         <v>45</v>
       </c>
-      <c r="F15">
-        <f>VLOOKUP(E15,Asset!A:D,4,FALSE)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -24727,12 +24681,9 @@
       <c r="E16" s="4">
         <v>47</v>
       </c>
-      <c r="F16">
-        <f>VLOOKUP(E16,Asset!A:D,4,FALSE)</f>
-        <v>5</v>
-      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:K16" xr:uid="{75DA7273-E739-C44B-8EA5-04AF4A472D36}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>